<commit_message>
reservations service finished, readme file with Prerequisites and Installation added
</commit_message>
<xml_diff>
--- a/reservations_service/international_names_with_rooms_1000.xlsx
+++ b/reservations_service/international_names_with_rooms_1000.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25fc7af92590d36d/Education/IT Arkitektur KEA/Tværfagligt projekt/hotel-kong-arthur-api/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25fc7af92590d36d/Education/IT Arkitektur KEA/Tværfagligt projekt/hotel-kong-arthur-api/reservations_service/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27FE6F6-0115-3744-B6DE-A82F947CE6E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -637,7 +637,7 @@
   <dimension ref="A1:G1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>